<commit_message>
report is improved to the final
</commit_message>
<xml_diff>
--- a/Bloomberg data_Source 2.xlsx
+++ b/Bloomberg data_Source 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snoorsalihi/Desktop/DataScience/Bloomberg-P-L-Analysis-and-Visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665DB60A-8681-BF48-881F-FAE3AADAAEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5370DFA-CBAB-1741-80B3-DA4776DCB737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="520" windowWidth="26480" windowHeight="15500" activeTab="1" xr2:uid="{790DDEEE-302A-4D12-A3D1-DF5E484623AD}"/>
+    <workbookView xWindow="6760" yWindow="2800" windowWidth="24080" windowHeight="15500" activeTab="1" xr2:uid="{790DDEEE-302A-4D12-A3D1-DF5E484623AD}"/>
   </bookViews>
   <sheets>
     <sheet name="IS source" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="155">
   <si>
     <t>Ticker</t>
   </si>
@@ -496,17 +496,27 @@
   </si>
   <si>
     <t>Adjustment</t>
+  </si>
+  <si>
+    <t>Gross Profit %</t>
+  </si>
+  <si>
+    <t>Other Operating Revenue</t>
+  </si>
+  <si>
+    <t>CAGR                   19-23%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="#,###;\(#,###\);\-"/>
+    <numFmt numFmtId="165" formatCode="#,###;\(#,###\);\-"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,8 +557,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,8 +612,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -611,12 +656,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -627,22 +682,40 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DB18C71D-3F96-4C76-AAE8-D1ACF701B155}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -956,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD42F68-042B-4357-ABDB-631263EB20BD}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -977,20 +1050,20 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -999,10 +1072,10 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
@@ -1011,19 +1084,19 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
@@ -1032,7 +1105,7 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1062,7 +1135,7 @@
       <c r="C7" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1149,7 +1222,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1829,7 +1902,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1861,7 +1934,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2093,7 +2166,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2125,7 +2198,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -3679,314 +3752,413 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A95765-7F90-D743-A132-631D0555C81E}">
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="20.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="0.33203125" style="7" customWidth="1"/>
+    <col min="4" max="8" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="B1" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="C1" s="10"/>
+    </row>
+    <row r="4" spans="2:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="B4" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="20" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="I4" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>10003.700000000001</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>10853.04</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>12462.05</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>12259.54</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>12087.66</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="I5" s="24">
+        <f>(H5/D5)^(1/4)-1</f>
+        <v>4.8444375275666696E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>2657.8</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>3169.28</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>3890.39</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>4337.26</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>4577.37</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="I6" s="24">
+        <f t="shared" ref="I6:I10" si="0">(H6/D6)^(1/4)-1</f>
+        <v>0.14557474425748995</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>1789.06</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>1883.79</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>2197.2199999999998</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>2540.89</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="19">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>2584.9</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="I7" s="24">
+        <f t="shared" si="0"/>
+        <v>9.6363857345664661E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="30">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>25.1</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="30">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="30">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="30">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="30">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="I8" s="28"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="17">
-        <f>SUM(D5:D7)</f>
-        <v>14450.56</v>
-      </c>
-      <c r="E9" s="17">
+      <c r="D9" s="19">
+        <f>SUM(D5:D8)</f>
+        <v>14475.66</v>
+      </c>
+      <c r="E9" s="19">
         <f>SUM(E5:E7)</f>
         <v>15906.11</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="19">
         <f>SUM(F5:F7)</f>
         <v>18549.66</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="19">
         <f>SUM(G5:G7)</f>
         <v>19137.690000000002</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="19">
         <f>SUM(H5:H7)</f>
         <v>19249.93</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="24">
+        <f>(H9/D9)^(1/4)-1</f>
+        <v>7.3860072753893835E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="14">
         <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C10,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>-7882.7606999999998</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="14">
         <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C10,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>-8291.3433999999997</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="14">
         <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C10,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>-9737.1097000000009</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C10,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>-9663.3541999999998</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C10,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>-9696.6934999999994</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <f>SUM(D9:D10)</f>
-        <v>6567.7992999999997</v>
-      </c>
-      <c r="E11" s="17">
-        <f t="shared" ref="E11:H11" si="0">SUM(E9:E10)</f>
+        <v>6592.8993</v>
+      </c>
+      <c r="E11" s="13">
+        <f>SUM(E9:E10)</f>
         <v>7614.7666000000008</v>
       </c>
-      <c r="F11" s="17">
-        <f t="shared" si="0"/>
+      <c r="F11" s="13">
+        <f>SUM(F9:F10)</f>
         <v>8812.550299999999</v>
       </c>
-      <c r="G11" s="17">
-        <f t="shared" si="0"/>
+      <c r="G11" s="13">
+        <f>SUM(G9:G10)</f>
         <v>9474.3358000000026</v>
       </c>
-      <c r="H11" s="17">
-        <f t="shared" si="0"/>
+      <c r="H11" s="13">
+        <f>SUM(H9:H10)</f>
         <v>9553.2365000000009</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="I11" s="24">
+        <f>(H11/D11)^(1/4)-1</f>
+        <v>9.7156351793897588E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34">
+        <f>D11/D9</f>
+        <v>0.45544723349401683</v>
+      </c>
+      <c r="E12" s="34">
+        <f t="shared" ref="E12:H12" si="1">E11/E9</f>
+        <v>0.47873217273110774</v>
+      </c>
+      <c r="F12" s="34">
+        <f t="shared" si="1"/>
+        <v>0.47507880467889974</v>
+      </c>
+      <c r="G12" s="34">
+        <f t="shared" si="1"/>
+        <v>0.49506161924453795</v>
+      </c>
+      <c r="H12" s="34">
+        <f t="shared" si="1"/>
+        <v>0.49627383060613733</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="18">
-        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C12,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
+      <c r="D13" s="14">
+        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C13,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>-6121.5848999999998</v>
       </c>
-      <c r="E12" s="18">
-        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C12,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
+      <c r="E13" s="14">
+        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C13,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>-6694.0990000000002</v>
       </c>
-      <c r="F12" s="18">
-        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C12,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
+      <c r="F13" s="14">
+        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C13,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>-7751.5357999999997</v>
       </c>
-      <c r="G12" s="18">
-        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C12,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
+      <c r="G13" s="14">
+        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C13,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>-8248.8911000000007</v>
       </c>
-      <c r="H12" s="18">
-        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C12,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
+      <c r="H13" s="14">
+        <f>-INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C13,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>-8215.6232</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="14">
+        <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C14,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
+        <v>259.36559999999997</v>
+      </c>
+      <c r="E14" s="14">
+        <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C14,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
+        <v>278.58909999999997</v>
+      </c>
+      <c r="F14" s="14">
+        <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C14,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
+        <v>265.94990000000001</v>
+      </c>
+      <c r="G14" s="14">
+        <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C14,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
+        <v>298.32310000000001</v>
+      </c>
+      <c r="H14" s="14">
+        <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C14,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
+        <v>328.09359999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="19">
-        <f>SUM(D11:D12)</f>
-        <v>446.21439999999984</v>
-      </c>
-      <c r="E13" s="19">
-        <f t="shared" ref="E13:H13" si="1">SUM(E11:E12)</f>
-        <v>920.66760000000068</v>
-      </c>
-      <c r="F13" s="19">
-        <f t="shared" si="1"/>
-        <v>1061.0144999999993</v>
-      </c>
-      <c r="G13" s="19">
-        <f t="shared" si="1"/>
-        <v>1225.4447000000018</v>
-      </c>
-      <c r="H13" s="19">
-        <f t="shared" si="1"/>
-        <v>1337.6133000000009</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+      <c r="D15" s="22">
+        <f>D11+D13+D14</f>
+        <v>730.68000000000018</v>
+      </c>
+      <c r="E15" s="22">
+        <f t="shared" ref="E15:H15" si="2">E11+E13+E14</f>
+        <v>1199.2567000000006</v>
+      </c>
+      <c r="F15" s="22">
+        <f t="shared" si="2"/>
+        <v>1326.9643999999994</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="2"/>
+        <v>1523.7678000000019</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="2"/>
+        <v>1665.7069000000008</v>
+      </c>
+      <c r="I15" s="25">
+        <f>(H15/D15)^(1/4)-1</f>
+        <v>0.22876219526653641</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="7">
-        <f>D13/D9</f>
-        <v>3.0878692590460152E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="20" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="36">
+        <f>D15/D9</f>
+        <v>5.0476454959566625E-2</v>
+      </c>
+      <c r="E16" s="36">
+        <f t="shared" ref="E16:H16" si="3">E15/E9</f>
+        <v>7.5395976766160958E-2</v>
+      </c>
+      <c r="F16" s="36">
+        <f t="shared" si="3"/>
+        <v>7.153578017063382E-2</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" si="3"/>
+        <v>7.9621302257482582E-2</v>
+      </c>
+      <c r="H16" s="36">
+        <f t="shared" si="3"/>
+        <v>8.6530543227949439E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
visulazation of P&L created
</commit_message>
<xml_diff>
--- a/Bloomberg data_Source 2.xlsx
+++ b/Bloomberg data_Source 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snoorsalihi/Desktop/DataScience/Bloomberg-P-L-Analysis-and-Visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5370DFA-CBAB-1741-80B3-DA4776DCB737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEE3073-1C2C-8C45-B671-3F2A5B1B84D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="2800" windowWidth="24080" windowHeight="15500" activeTab="1" xr2:uid="{790DDEEE-302A-4D12-A3D1-DF5E484623AD}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="24080" windowHeight="15500" activeTab="1" xr2:uid="{790DDEEE-302A-4D12-A3D1-DF5E484623AD}"/>
   </bookViews>
   <sheets>
     <sheet name="IS source" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,30 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IS source'!$A$9:$J$80</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'P&amp;L Statement'!$D$15:$H$15</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'P&amp;L Statement'!$D$4:$H$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'P&amp;L Statement'!$D$7:$H$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'P&amp;L Statement'!$D$8:$H$8</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'P&amp;L Statement'!$D$15:$H$15</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'P&amp;L Statement'!$D$4:$H$4</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'P&amp;L Statement'!$D$5:$H$5</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'P&amp;L Statement'!$D$6:$H$6</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'P&amp;L Statement'!$D$7:$H$7</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'P&amp;L Statement'!$D$8:$H$8</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'P&amp;L Statement'!$D$15:$H$15</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'P&amp;L Statement'!$D$4:$H$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'P&amp;L Statement'!$D$5:$H$5</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'P&amp;L Statement'!$D$5:$H$5</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'P&amp;L Statement'!$D$6:$H$6</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'P&amp;L Statement'!$D$7:$H$7</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'P&amp;L Statement'!$D$8:$H$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'P&amp;L Statement'!$D$6:$H$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'P&amp;L Statement'!$D$7:$H$7</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'P&amp;L Statement'!$D$8:$H$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'P&amp;L Statement'!$D$15:$H$15</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'P&amp;L Statement'!$D$4:$H$4</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'P&amp;L Statement'!$D$5:$H$5</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'P&amp;L Statement'!$D$6:$H$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -514,7 +538,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,###;\(#,###\);\-"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -671,7 +695,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -688,29 +712,25 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,6 +748,1585 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Adidas Revenue: FY2019-FY2023</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wholesale</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'P&amp;L Statement'!$D$4:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY 2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY 2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY 2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P&amp;L Statement'!$D$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,###;\(#,###\);\-</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10003.700000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10853.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12462.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12259.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12087.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD03-1444-AF70-F25261A3A0BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Retail</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'P&amp;L Statement'!$D$4:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY 2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY 2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY 2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P&amp;L Statement'!$D$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,###;\(#,###\);\-</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2657.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3169.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3890.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4337.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4577.37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DD03-1444-AF70-F25261A3A0BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Other Businesses</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'P&amp;L Statement'!$D$4:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY 2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY 2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY 2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P&amp;L Statement'!$D$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,###;\(#,###\);\-</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1789.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1883.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2197.2199999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2540.89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2584.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DD03-1444-AF70-F25261A3A0BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Adjustment</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'P&amp;L Statement'!$D$4:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY 2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY 2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY 2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P&amp;L Statement'!$D$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,###;\(#,###\);\-</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DD03-1444-AF70-F25261A3A0BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:overlap val="100"/>
+        <c:axId val="2077348735"/>
+        <c:axId val="2085886223"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>EBIT%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'P&amp;L Statement'!$D$4:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY 2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY 2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY 2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P&amp;L Statement'!$D$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0476454959566625E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5395976766160958E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.153578017063382E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9621302257482582E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6530543227949439E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD03-1444-AF70-F25261A3A0BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="74307488"/>
+        <c:axId val="34789904"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2077348735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2085886223"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2085886223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25000"/>
+          <c:min val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>$ in million</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="0" i="0" u="none" strike="noStrike" cap="all" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,###;\(#,###\);\-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2077348735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="34789904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1"/>
+                  <a:t>EBIT%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74307488"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.02"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="74307488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34789904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="225">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A157490-4C83-A8A9-7634-D798FA4C49B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,20 +2649,20 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -1072,10 +2671,10 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
@@ -1084,19 +2683,19 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
@@ -3755,7 +5354,7 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3768,188 +5367,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="26" t="s">
         <v>144</v>
       </c>
       <c r="C1" s="10"/>
     </row>
     <row r="4" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="20" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>10003.700000000001</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>10853.04</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>12462.05</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>12259.54</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C5,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>12087.66</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="21">
         <f>(H5/D5)^(1/4)-1</f>
         <v>4.8444375275666696E-2</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>2657.8</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>3169.28</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>3890.39</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>4337.26</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C6,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>4577.37</v>
       </c>
-      <c r="I6" s="24">
-        <f t="shared" ref="I6:I10" si="0">(H6/D6)^(1/4)-1</f>
+      <c r="I6" s="21">
+        <f t="shared" ref="I6:I7" si="0">(H6/D6)^(1/4)-1</f>
         <v>0.14557474425748995</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>1789.06</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>1883.79</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>2197.2199999999998</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>2540.89</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="14">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C7,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>2584.9</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="21">
         <f t="shared" si="0"/>
         <v>9.6363857345664661E-2</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="25">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!D$4,'IS source'!$9:$9,0))</f>
         <v>25.1</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="25">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!E$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="25">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!F$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="25">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!G$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="25">
         <f>INDEX('IS source'!$1:$1048576,MATCH('P&amp;L Statement'!$C8,'IS source'!$A:$A,0),MATCH('P&amp;L Statement'!H$4,'IS source'!$9:$9,0))</f>
         <v>0</v>
       </c>
-      <c r="I8" s="28"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="14">
         <f>SUM(D5:D8)</f>
         <v>14475.66</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="14">
         <f>SUM(E5:E7)</f>
         <v>15906.11</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="14">
         <f>SUM(F5:F7)</f>
         <v>18549.66</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="14">
         <f>SUM(G5:G7)</f>
         <v>19137.690000000002</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="14">
         <f>SUM(H5:H7)</f>
         <v>19249.93</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="21">
         <f>(H9/D9)^(1/4)-1</f>
         <v>7.3860072753893835E-2</v>
       </c>
@@ -4009,33 +5608,33 @@
         <f>SUM(H9:H10)</f>
         <v>9553.2365000000009</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="21">
         <f>(H11/D11)^(1/4)-1</f>
         <v>9.7156351793897588E-2</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34">
+      <c r="C12" s="28"/>
+      <c r="D12" s="29">
         <f>D11/D9</f>
         <v>0.45544723349401683</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="29">
         <f t="shared" ref="E12:H12" si="1">E11/E9</f>
         <v>0.47873217273110774</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="29">
         <f t="shared" si="1"/>
         <v>0.47507880467889974</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="29">
         <f t="shared" si="1"/>
         <v>0.49506161924453795</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="29">
         <f t="shared" si="1"/>
         <v>0.49627383060613733</v>
       </c>
@@ -4100,56 +5699,56 @@
       <c r="B15" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="19">
         <f>D11+D13+D14</f>
         <v>730.68000000000018</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="19">
         <f t="shared" ref="E15:H15" si="2">E11+E13+E14</f>
         <v>1199.2567000000006</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="19">
         <f t="shared" si="2"/>
         <v>1326.9643999999994</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="19">
         <f t="shared" si="2"/>
         <v>1523.7678000000019</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <f t="shared" si="2"/>
         <v>1665.7069000000008</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="22">
         <f>(H15/D15)^(1/4)-1</f>
         <v>0.22876219526653641</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36">
+      <c r="C16" s="27"/>
+      <c r="D16" s="30">
         <f>D15/D9</f>
         <v>5.0476454959566625E-2</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="30">
         <f t="shared" ref="E16:H16" si="3">E15/E9</f>
         <v>7.5395976766160958E-2</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="30">
         <f t="shared" si="3"/>
         <v>7.153578017063382E-2</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="30">
         <f t="shared" si="3"/>
         <v>7.9621302257482582E-2</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="30">
         <f t="shared" si="3"/>
         <v>8.6530543227949439E-2</v>
       </c>
@@ -4162,5 +5761,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>